<commit_message>
Added code for testcase
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/MystoreTestData.xlsx
+++ b/src/test/resources/testdata/MystoreTestData.xlsx
@@ -1,13 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sarang\eclipse-workspace\MyStore\src\test\resources\testdata\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A72254A-A0F1-4592-9BCE-1A402550213A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="newuserinfo" sheetId="1" r:id="rId1"/>
+    <sheet name="usercredentials" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -18,12 +25,133 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+  <si>
+    <t>UserEmailId</t>
+  </si>
+  <si>
+    <t>CustomerFirstName</t>
+  </si>
+  <si>
+    <t>CustomerLastName</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>CustomerGender</t>
+  </si>
+  <si>
+    <t>BirthDay</t>
+  </si>
+  <si>
+    <t>BirthMonth</t>
+  </si>
+  <si>
+    <t>BirthYear</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>CompanyName</t>
+  </si>
+  <si>
+    <t>AddressLine1</t>
+  </si>
+  <si>
+    <t>AddressLine2</t>
+  </si>
+  <si>
+    <t>CityName</t>
+  </si>
+  <si>
+    <t>StateName</t>
+  </si>
+  <si>
+    <t>ZipCodeNumber</t>
+  </si>
+  <si>
+    <t>AdditionalInfo</t>
+  </si>
+  <si>
+    <t>HomePhoneNumber</t>
+  </si>
+  <si>
+    <t>MobileNumber</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>Ellis</t>
+  </si>
+  <si>
+    <t>hi there</t>
+  </si>
+  <si>
+    <t>01002</t>
+  </si>
+  <si>
+    <t>Alaska</t>
+  </si>
+  <si>
+    <t>DownTown Road</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>richard</t>
+  </si>
+  <si>
+    <t>Unicorn Techno Pvt Ltd</t>
+  </si>
+  <si>
+    <t>thomasprichard@gmail.com</t>
+  </si>
+  <si>
+    <t>thomasp</t>
+  </si>
+  <si>
+    <t>b@TqR2UW7vq@RuJ</t>
+  </si>
+  <si>
+    <t>1772  Backer Street, PO Box 23</t>
+  </si>
+  <si>
+    <t>479-221-1655</t>
+  </si>
+  <si>
+    <t>208-207-9548</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0;[Red]0"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -46,13 +174,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -330,13 +464,189 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.33203125" style="2" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2">
+        <v>1985</v>
+      </c>
+      <c r="I2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" t="s">
+        <v>32</v>
+      </c>
+      <c r="M2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O2" t="s">
+        <v>23</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D159E5BA-6AA6-4E93-8654-F78CF3413A29}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="23.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>